<commit_message>
Another page and a maybe better matching.
</commit_message>
<xml_diff>
--- a/changed.xlsx
+++ b/changed.xlsx
@@ -1447,137 +1447,104 @@
       <c r="F3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
-        <f>VLOOKUP(G1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="H3" s="1">
-        <f>VLOOKUP(H1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="I3" s="1">
-        <f>VLOOKUP(I1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="J3" s="1">
-        <f>VLOOKUP(J1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="K3" s="1">
-        <f>VLOOKUP(K1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="L3" s="1">
-        <f>VLOOKUP(L1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="M3" s="1">
-        <f>VLOOKUP(M1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="N3" s="1">
-        <f>VLOOKUP(N1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="O3" s="1">
-        <f>VLOOKUP(O1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="P3" s="1">
-        <f>VLOOKUP(P1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="Q3" s="1">
-        <f>VLOOKUP(Q1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="R3" s="1">
-        <f>VLOOKUP(R1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="S3" s="1">
-        <f>VLOOKUP(S1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="T3" s="1">
-        <f>VLOOKUP(T1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="U3" s="1">
-        <f>VLOOKUP(U1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="V3" s="1">
-        <f>VLOOKUP(V1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="W3" s="1">
-        <f>VLOOKUP(W1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="X3" s="1">
-        <f>VLOOKUP(X1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="Y3" s="1">
-        <f>VLOOKUP(Y1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="Z3" s="1">
-        <f>VLOOKUP(Z1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AA3" s="1">
-        <f>VLOOKUP(AA1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AB3" s="1">
-        <f>VLOOKUP(AB1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AC3" s="1">
-        <f>VLOOKUP(AC1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AD3" s="1">
-        <f>VLOOKUP(AD1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AE3" s="1">
-        <f>VLOOKUP(AE1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AF3" s="1">
-        <f>VLOOKUP(AF1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AG3" s="1">
-        <f>VLOOKUP(AG1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AH3" s="1">
-        <f>VLOOKUP(AH1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AI3" s="1">
-        <f>VLOOKUP(AI1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AJ3" s="1">
-        <f>VLOOKUP(AJ1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AK3" s="1">
-        <f>VLOOKUP(AK1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AL3" s="1">
-        <f>VLOOKUP(AL1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
-      </c>
-      <c r="AM3" s="1">
-        <f>VLOOKUP(AM1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>
-        <v/>
+      <c r="G3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="P3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="X3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="AN3" s="1">
         <f>VLOOKUP(AN1,'Code Plan'!$A$1:$H$111,8,FALSE)</f>

</xml_diff>